<commit_message>
deadline clean up issues fixed
</commit_message>
<xml_diff>
--- a/access_scholarships.xlsx
+++ b/access_scholarships.xlsx
@@ -442,7 +442,7 @@
         <v>2500</v>
       </c>
       <c r="C2" t="str">
-        <v>Scholarship Points $2,500 Scholarship</v>
+        <v>N/a</v>
       </c>
       <c r="D2" t="str">
         <v>The Scholarship Points $2,500 scholarship is awarded to one lucky student each month of the year. There is no essay or minimum GPA required!</v>
@@ -474,7 +474,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="str">
-        <v>North Carolina Nurses Association Scholarships</v>
+        <v>N/a</v>
       </c>
       <c r="D3" t="str">
         <v>The North Carolina Foundation for Nursing is proud to sponsor a number of scholarship opportunities for nurses and nursing students.</v>
@@ -506,7 +506,7 @@
         <v>1000</v>
       </c>
       <c r="C4" t="str">
-        <v>Rustic Pathways Global Perspectives Scholarship</v>
+        <v>08/01/2025</v>
       </c>
       <c r="D4" t="str">
         <v>Rustic Pathways empowers students to positively impact lives and communities around the world through its innovative and responsible travel experiences. Rustic Pathways is offering a $1,000 scholarship to two high school or college students attending an accredited college or university in the upcoming fall. Four students will also receive prizes of $250 each.</v>
@@ -538,7 +538,7 @@
         <v>0</v>
       </c>
       <c r="C5" t="str">
-        <v>Duke and Dutchess of Cambridge Scholarship</v>
+        <v>08/01/2030</v>
       </c>
       <c r="D5" t="str">
         <v>To commemorate the Duke and Duchess of Cambridge’s Royal Visit to Alberta in July 2011, the Government of Alberta established the Duke and Duchess of Cambridge Scholarship. The scholarship recognizes the exceptional educational achievements of Advancing Futures students who have been in government care.</v>
@@ -570,7 +570,7 @@
         <v>10000</v>
       </c>
       <c r="C6" t="str">
-        <v>CollegExpress $10,000 Scholarship</v>
+        <v>12/01/2031</v>
       </c>
       <c r="D6" t="str">
         <v>The CollegExpress $10,000 Scholarship is award annually from a pool of registrations . There is no essay required. Simply sign up to be automatically entered into the scholarship.</v>
@@ -602,7 +602,7 @@
         <v>500</v>
       </c>
       <c r="C7" t="str">
-        <v>The ANTSHE Board of Directors Scholarship</v>
+        <v>08/01/2030</v>
       </c>
       <c r="D7" t="str">
         <v>The ANTSHE Board Scholarship is awarded to a non-traditional student that demonstrates academic achievement and who contributes to the adult learner program at their college/university. Must be a non-traditional undergraduate student member of ANTSHE. Applicant must be considered a non-traditional student, Be enrolled as a full-time student in a four-year program of study at an accredited college or university in an undergraduate program, and demonstrate their contribution to their college and community. May award $500 up to full tuition.</v>
@@ -634,7 +634,7 @@
         <v>500</v>
       </c>
       <c r="C8" t="str">
-        <v>The Founder’s Scholarship</v>
+        <v>08/01/2030</v>
       </c>
       <c r="D8" t="str">
         <v>The Founder’s Scholarship is awarded to a non-traditional student that demonstrates need and achievement. Must be a non-traditional undergraduate student member of ANTSHE. Applicant contributes to the enrichment of their college and/or local community and demonstrates their continued contribution to their college and community. Applicant must be considered a non-traditional student, Be enrolled as a full-time student in a four-year program of study at an accredited college or university in an undergraduate program, and demonstrate their contribution to their college and community. May award $500 up to full tuition.</v>
@@ -666,7 +666,7 @@
         <v>1000</v>
       </c>
       <c r="C9" t="str">
-        <v>Career Colleges and Schools of Texas Scholarship Program</v>
+        <v>08/01/2031</v>
       </c>
       <c r="D9" t="str">
         <v>Members of the Career Colleges &amp; Schools of Texas (CCST) are proud to finance a $1,000 scholarship for graduating seniors.</v>
@@ -698,7 +698,7 @@
         <v>25000</v>
       </c>
       <c r="C10" t="str">
-        <v>Be Bold Scholarship (No Essay!)</v>
+        <v>N/a</v>
       </c>
       <c r="D10" t="str">
         <v>About the “Be Bold” Scholarship</v>
@@ -730,7 +730,7 @@
         <v>500</v>
       </c>
       <c r="C11" t="str">
-        <v>Morgan Franklin Foundation Financial Independence Scholarship</v>
+        <v>08/01/2031</v>
       </c>
       <c r="D11" t="str">
         <v>Award: $500 (one-time)</v>
@@ -762,7 +762,7 @@
         <v>40000</v>
       </c>
       <c r="C12" t="str">
-        <v>Oregon Historic Trails Fund</v>
+        <v>08/01/2031</v>
       </c>
       <c r="D12" t="str">
         <v>Each fall, the Oregon Historic Trails Fund awards grants to support projects that interpret, preserve or maintain Oregon’s trail-related resources. Grants may also be awarded for marketing, education, advocacy and research relating to historic trails. Kindly visit the scholarship site for the comprehensive list of requirements and more information.</v>
@@ -794,7 +794,7 @@
         <v>3000</v>
       </c>
       <c r="C13" t="str">
-        <v>Secular Student Alliance Scholarships</v>
+        <v>08/01/2031</v>
       </c>
       <c r="D13" t="str">
         <v>The scholarships are available to SSA student members enrolled in high school or college in the United States and are designed to support students who in addition to pursuing excellence in their academic studies are also activists for secular values on their campus and/or in their community.</v>
@@ -826,7 +826,7 @@
         <v>1500</v>
       </c>
       <c r="C14" t="str">
-        <v>North Carolina Vending Association Academic Scholarships</v>
+        <v>09/01/2001</v>
       </c>
       <c r="D14" t="str">
         <v>The North Carolina Vending Association, the organization representing the vending and food service industry in the state, was formed in 1955 and is the oldest independent vending association in the nation. In an effort to contribute to the communities that have made the industry what it is, NCVA formed a scholarship. A $1,500 scholarship, based on academics, character and financial need is awarded to a deserving student (student must be affiliated with/related to a person from the vending industry and a CURRENT Member of NCVA) from North Carolina each year. It is with great pleasure that we offer this opportunity to you. We wish for each of you a rewarding educational experience and a successful career.</v>

</xml_diff>